<commit_message>
Working with trend market using ma N periods
</commit_message>
<xml_diff>
--- a/FTMUSDT_5m_556159355.xlsx
+++ b/FTMUSDT_5m_556159355.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,16 +572,16 @@
         <v>1025.788854251094</v>
       </c>
       <c r="G3" t="n">
-        <v>2.314940239043825</v>
+        <v>2.320718921617573</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J3" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K3" t="n">
         <v>1.02</v>
@@ -591,11 +591,7 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>-0.0033800000</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="n">
         <v>2.325150505050505</v>
       </c>
@@ -605,16 +601,16 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2841</v>
+        <v>2320</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44571.86458333334</v>
+        <v>44570.05555555555</v>
       </c>
       <c r="C4" t="n">
-        <v>1641847799999</v>
+        <v>1641691499999</v>
       </c>
       <c r="D4" t="n">
-        <v>2.239</v>
+        <v>2.3184</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -622,19 +618,19 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>457.6881982001063</v>
+        <v>442.0134039725837</v>
       </c>
       <c r="G4" t="n">
-        <v>2.247956</v>
+        <v>2.3218776</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J4" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K4" t="n">
         <v>1.02</v>
@@ -644,30 +640,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>-0.0162909091</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
-        <v>2.223918181818182</v>
+        <v>2.284191919191919</v>
       </c>
       <c r="O4" t="n">
-        <v>59.11237016052877</v>
+        <v>63.65946632782724</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3003</v>
+        <v>2394</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44572.42708333334</v>
+        <v>44570.3125</v>
       </c>
       <c r="C5" t="n">
-        <v>1641896399999</v>
+        <v>1641713699999</v>
       </c>
       <c r="D5" t="n">
-        <v>2.3217</v>
+        <v>2.3422</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -675,19 +667,19 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1061.614689761187</v>
+        <v>1034.283794784586</v>
       </c>
       <c r="G5" t="n">
-        <v>2.312450199203187</v>
+        <v>2.338691962056914</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J5" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K5" t="n">
         <v>1.02</v>
@@ -697,30 +689,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0.0002617857</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="n">
-        <v>2.322518181818182</v>
+        <v>2.3519</v>
       </c>
       <c r="O5" t="n">
-        <v>53.08641975308638</v>
+        <v>44.89194499017694</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6196</v>
+        <v>2463</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44583.51388888889</v>
+        <v>44570.55208333334</v>
       </c>
       <c r="C6" t="n">
-        <v>1642854299999</v>
+        <v>1641734399999</v>
       </c>
       <c r="D6" t="n">
-        <v>2.0501</v>
+        <v>2.3267</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -728,19 +716,19 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>517.3181375284281</v>
+        <v>444.0840366501907</v>
       </c>
       <c r="G6" t="n">
-        <v>2.0583004</v>
+        <v>2.33019005</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J6" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K6" t="n">
         <v>1.02</v>
@@ -750,30 +738,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>-0.0151706015</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
-        <v>2.034118181818182</v>
+        <v>2.32089191919192</v>
       </c>
       <c r="O6" t="n">
-        <v>60.31183557760453</v>
+        <v>59.55143078112924</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>6507</v>
+        <v>2578</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44584.59375</v>
+        <v>44570.95138888889</v>
       </c>
       <c r="C7" t="n">
-        <v>1642947599999</v>
+        <v>1641768899999</v>
       </c>
       <c r="D7" t="n">
-        <v>2.2236</v>
+        <v>2.4077</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -781,19 +765,19 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1149.308610608213</v>
+        <v>1068.221135042664</v>
       </c>
       <c r="G7" t="n">
-        <v>2.214741035856574</v>
+        <v>2.404093859211183</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J7" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K7" t="n">
         <v>1.02</v>
@@ -803,30 +787,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>-0.0065815385</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
-        <v>2.24129494949495</v>
+        <v>2.411665656565657</v>
       </c>
       <c r="O7" t="n">
-        <v>34.1661824520628</v>
+        <v>47.06982543640902</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6799</v>
+        <v>2841</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44585.60763888889</v>
+        <v>44571.86458333334</v>
       </c>
       <c r="C8" t="n">
-        <v>1643035199999</v>
+        <v>1641847799999</v>
       </c>
       <c r="D8" t="n">
-        <v>2.0361</v>
+        <v>2.239</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -834,19 +814,19 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>563.9016796578787</v>
+        <v>476.6207046906291</v>
       </c>
       <c r="G8" t="n">
-        <v>2.0442444</v>
+        <v>2.2423585</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J8" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K8" t="n">
         <v>1.02</v>
@@ -856,30 +836,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>-0.0112160845</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="n">
-        <v>1.99029494949495</v>
+        <v>2.223918181818182</v>
       </c>
       <c r="O8" t="n">
-        <v>78.22899041173159</v>
+        <v>59.11237016052877</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>6922</v>
+        <v>3003</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44586.03472222222</v>
+        <v>44572.42708333334</v>
       </c>
       <c r="C9" t="n">
-        <v>1643072099999</v>
+        <v>1641896399999</v>
       </c>
       <c r="D9" t="n">
-        <v>2.1788</v>
+        <v>2.3217</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -887,19 +863,19 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1227.628979638586</v>
+        <v>1105.570290080233</v>
       </c>
       <c r="G9" t="n">
-        <v>2.17011952191235</v>
+        <v>2.318222666000998</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J9" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K9" t="n">
         <v>1.02</v>
@@ -909,30 +885,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>-0.0067357423</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="n">
-        <v>2.190483838383838</v>
+        <v>2.322518181818182</v>
       </c>
       <c r="O9" t="n">
-        <v>26.11111111111121</v>
+        <v>53.08641975308638</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>7595</v>
+        <v>6087</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44588.37152777778</v>
+        <v>44583.13541666666</v>
       </c>
       <c r="C10" t="n">
-        <v>1643273999999</v>
+        <v>1642821599999</v>
       </c>
       <c r="D10" t="n">
-        <v>2.166</v>
+        <v>2.3152</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -940,19 +912,19 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>566.2060574726877</v>
+        <v>477.049755179113</v>
       </c>
       <c r="G10" t="n">
-        <v>2.174664</v>
+        <v>2.3186728</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J10" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K10" t="n">
         <v>1.02</v>
@@ -962,30 +934,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>-0.0053691651</t>
-        </is>
-      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>2.14459797979798</v>
+        <v>2.308889898989899</v>
       </c>
       <c r="O10" t="n">
-        <v>61.04089219330849</v>
+        <v>63.51791530944619</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>7677</v>
+        <v>7152</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44588.65625</v>
+        <v>44586.83333333334</v>
       </c>
       <c r="C11" t="n">
-        <v>1643298599999</v>
+        <v>1643141099999</v>
       </c>
       <c r="D11" t="n">
-        <v>2.1824</v>
+        <v>2.3944</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -993,19 +961,19 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1234.688099828394</v>
+        <v>1141.247933800868</v>
       </c>
       <c r="G11" t="n">
-        <v>2.173705179282868</v>
+        <v>2.390813779331003</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J11" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K11" t="n">
         <v>1.02</v>
@@ -1015,30 +983,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>-0.0036254677</t>
-        </is>
-      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
-        <v>2.18390707070707</v>
+        <v>2.403896969696969</v>
       </c>
       <c r="O11" t="n">
-        <v>34.19243986254298</v>
+        <v>32.7645051194539</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>7777</v>
+        <v>7246</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44589.00347222222</v>
+        <v>44587.15972222222</v>
       </c>
       <c r="C12" t="n">
-        <v>1643328599999</v>
+        <v>1643169299999</v>
       </c>
       <c r="D12" t="n">
-        <v>2.1055</v>
+        <v>2.3395</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1046,19 +1010,19 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>585.8249285833123</v>
+        <v>487.3295949788139</v>
       </c>
       <c r="G12" t="n">
-        <v>2.113922</v>
+        <v>2.34300925</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J12" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K12" t="n">
         <v>1.02</v>
@@ -1068,30 +1032,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>-0.0037411909</t>
-        </is>
-      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>2.085350505050505</v>
+        <v>2.337111111111111</v>
       </c>
       <c r="O12" t="n">
-        <v>78.92918825561317</v>
+        <v>63.35807050092755</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>8094</v>
+        <v>7344</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44590.10416666666</v>
+        <v>44587.5</v>
       </c>
       <c r="C13" t="n">
-        <v>1643423699999</v>
+        <v>1643198699999</v>
       </c>
       <c r="D13" t="n">
-        <v>2.1166</v>
+        <v>2.3492</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1099,19 +1059,19 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1238.957043839439</v>
+        <v>1143.83468452423</v>
       </c>
       <c r="G13" t="n">
-        <v>2.108167330677291</v>
+        <v>2.345681477783325</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J13" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K13" t="n">
         <v>1.02</v>
@@ -1121,30 +1081,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>-0.0032351371</t>
-        </is>
-      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
-        <v>2.119122222222222</v>
+        <v>2.355535353535354</v>
       </c>
       <c r="O13" t="n">
-        <v>40.93376764386522</v>
+        <v>37.24539282250248</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>8733</v>
+        <v>7595</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44592.32291666666</v>
+        <v>44588.37152777778</v>
       </c>
       <c r="C14" t="n">
-        <v>1643615399999</v>
+        <v>1643273999999</v>
       </c>
       <c r="D14" t="n">
-        <v>1.9487</v>
+        <v>2.166</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1152,19 +1108,19 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>635.1511600408805</v>
+        <v>527.5585196071589</v>
       </c>
       <c r="G14" t="n">
-        <v>1.9564948</v>
+        <v>2.169249</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J14" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K14" t="n">
         <v>1.02</v>
@@ -1174,30 +1130,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>-0.0042826424</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="n">
-        <v>1.948617171717172</v>
+        <v>2.14459797979798</v>
       </c>
       <c r="O14" t="n">
-        <v>72.81105990783425</v>
+        <v>61.04089219330849</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>8911</v>
+        <v>7677</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44592.94097222222</v>
+        <v>44588.65625</v>
       </c>
       <c r="C15" t="n">
-        <v>1643668799999</v>
+        <v>1643298599999</v>
       </c>
       <c r="D15" t="n">
-        <v>2.042</v>
+        <v>2.1824</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1205,19 +1157,19 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1295.978668803478</v>
+        <v>1150.343713190663</v>
       </c>
       <c r="G15" t="n">
-        <v>2.033864541832669</v>
+        <v>2.179131303045432</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J15" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K15" t="n">
         <v>1.02</v>
@@ -1227,30 +1179,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>-0.0040215079</t>
-        </is>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>2.046781818181818</v>
+        <v>2.18390707070707</v>
       </c>
       <c r="O15" t="n">
-        <v>36.63366336633633</v>
+        <v>34.19243986254298</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>9568</v>
+        <v>7777</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44595.22222222222</v>
+        <v>44589.00347222222</v>
       </c>
       <c r="C16" t="n">
-        <v>1643865899999</v>
+        <v>1643328599999</v>
       </c>
       <c r="D16" t="n">
-        <v>1.9263</v>
+        <v>2.1055</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1258,19 +1206,19 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>672.1090764459445</v>
+        <v>545.8058790068897</v>
       </c>
       <c r="G16" t="n">
-        <v>1.9340052</v>
+        <v>2.10865825</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J16" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K16" t="n">
         <v>1.02</v>
@@ -1280,30 +1228,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>-0.0045182696</t>
-        </is>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="n">
-        <v>1.917884848484849</v>
+        <v>2.085350505050505</v>
       </c>
       <c r="O16" t="n">
-        <v>61.165048543689</v>
+        <v>78.92918825561317</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>9847</v>
+        <v>8084</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44596.19097222222</v>
+        <v>44590.06944444445</v>
       </c>
       <c r="C17" t="n">
-        <v>1643949599999</v>
+        <v>1643420699999</v>
       </c>
       <c r="D17" t="n">
-        <v>1.9358</v>
+        <v>2.1091</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1311,19 +1255,19 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1300.068750184059</v>
+        <v>1150.159179413431</v>
       </c>
       <c r="G17" t="n">
-        <v>1.92808764940239</v>
+        <v>2.105941088367449</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J17" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K17" t="n">
         <v>1.02</v>
@@ -1333,30 +1277,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>-0.0046489246</t>
-        </is>
-      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
-        <v>1.937238383838384</v>
+        <v>2.113860606060606</v>
       </c>
       <c r="O17" t="n">
-        <v>41.47157190635448</v>
+        <v>32.42320819112621</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>12257</v>
+        <v>8733</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44604.55902777778</v>
+        <v>44592.32291666666</v>
       </c>
       <c r="C18" t="n">
-        <v>1644672599999</v>
+        <v>1643615399999</v>
       </c>
       <c r="D18" t="n">
-        <v>1.9253</v>
+        <v>1.9487</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1364,19 +1304,19 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>674.5804334328094</v>
+        <v>589.62894691834</v>
       </c>
       <c r="G18" t="n">
-        <v>1.9330012</v>
+        <v>1.95162305</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J18" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K18" t="n">
         <v>1.02</v>
@@ -1386,30 +1326,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>-0.0046881060</t>
-        </is>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
-        <v>1.925141414141414</v>
+        <v>1.948617171717172</v>
       </c>
       <c r="O18" t="n">
-        <v>67.10526315789485</v>
+        <v>72.81105990783425</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>12365</v>
+        <v>8911</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44604.93402777778</v>
+        <v>44592.94097222222</v>
       </c>
       <c r="C19" t="n">
-        <v>1644704999999</v>
+        <v>1643668799999</v>
       </c>
       <c r="D19" t="n">
-        <v>1.937</v>
+        <v>2.042</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1417,19 +1353,19 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1305.662299559352</v>
+        <v>1203.02230960725</v>
       </c>
       <c r="G19" t="n">
-        <v>1.929282868525896</v>
+        <v>2.038941587618572</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J19" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K19" t="n">
         <v>1.02</v>
@@ -1439,30 +1375,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>-0.0045708462</t>
-        </is>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="n">
-        <v>1.93909595959596</v>
+        <v>2.046781818181818</v>
       </c>
       <c r="O19" t="n">
-        <v>44.35897435897441</v>
+        <v>36.63366336633633</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>12754</v>
+        <v>9568</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44606.28472222222</v>
+        <v>44595.22222222222</v>
       </c>
       <c r="C20" t="n">
-        <v>1644821699999</v>
+        <v>1643865899999</v>
       </c>
       <c r="D20" t="n">
-        <v>1.8682</v>
+        <v>1.9263</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1470,19 +1402,19 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>698.1895239979708</v>
+        <v>623.90086574535</v>
       </c>
       <c r="G20" t="n">
-        <v>1.8756728</v>
+        <v>1.92918945</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J20" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K20" t="n">
         <v>1.02</v>
@@ -1492,30 +1424,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>-0.0046786130</t>
-        </is>
-      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
-        <v>1.858665656565657</v>
+        <v>1.917884848484849</v>
       </c>
       <c r="O20" t="n">
-        <v>64.40129449838199</v>
+        <v>61.165048543689</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>12898</v>
+        <v>9840</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44606.78472222222</v>
+        <v>44596.16666666666</v>
       </c>
       <c r="C21" t="n">
-        <v>1644864899999</v>
+        <v>1643947499999</v>
       </c>
       <c r="D21" t="n">
-        <v>1.916</v>
+        <v>1.9301</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1523,19 +1451,19 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1336.731127980112</v>
+        <v>1203.1910609751</v>
       </c>
       <c r="G21" t="n">
-        <v>1.908366533864542</v>
+        <v>1.927209186220669</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J21" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K21" t="n">
         <v>1.02</v>
@@ -1545,30 +1473,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>-0.0044797942</t>
-        </is>
-      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
-        <v>1.917948484848485</v>
+        <v>1.93529595959596</v>
       </c>
       <c r="O21" t="n">
-        <v>31.6017316017313</v>
+        <v>36.08695652173925</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>14115</v>
+        <v>12257</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44611.01041666666</v>
+        <v>44604.55902777778</v>
       </c>
       <c r="C22" t="n">
-        <v>1645229999999</v>
+        <v>1644672599999</v>
       </c>
       <c r="D22" t="n">
-        <v>1.8763</v>
+        <v>1.9253</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1576,19 +1500,19 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>711.7174507646554</v>
+        <v>624.312481397737</v>
       </c>
       <c r="G22" t="n">
-        <v>1.8838052</v>
+        <v>1.92818795</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J22" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K22" t="n">
         <v>1.02</v>
@@ -1598,30 +1522,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>-0.0044287717</t>
-        </is>
-      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
-        <v>1.873607070707071</v>
+        <v>1.925141414141414</v>
       </c>
       <c r="O22" t="n">
-        <v>63.22314049586774</v>
+        <v>67.10526315789485</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>14213</v>
+        <v>12361</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44611.35069444445</v>
+        <v>44604.92013888889</v>
       </c>
       <c r="C23" t="n">
-        <v>1645259399999</v>
+        <v>1644703799999</v>
       </c>
       <c r="D23" t="n">
-        <v>1.888</v>
+        <v>1.93</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1629,19 +1549,19 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1342.722547043669</v>
+        <v>1203.923089097632</v>
       </c>
       <c r="G23" t="n">
-        <v>1.880478087649402</v>
+        <v>1.927109335996006</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J23" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K23" t="n">
         <v>1.02</v>
@@ -1651,30 +1571,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>-0.0042539260</t>
-        </is>
-      </c>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="n">
-        <v>1.889446464646465</v>
+        <v>1.938080808080808</v>
       </c>
       <c r="O23" t="n">
-        <v>24.09638554216809</v>
+        <v>34.60490463215265</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>14305</v>
+        <v>12754</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44611.67013888889</v>
+        <v>44606.28472222222</v>
       </c>
       <c r="C24" t="n">
-        <v>1645286999999</v>
+        <v>1644821699999</v>
       </c>
       <c r="D24" t="n">
-        <v>1.8669</v>
+        <v>1.8682</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1682,19 +1598,19 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>718.5070894249492</v>
+        <v>643.7855246267932</v>
       </c>
       <c r="G24" t="n">
-        <v>1.8743676</v>
+        <v>1.8710023</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J24" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K24" t="n">
         <v>1.02</v>
@@ -1704,30 +1620,26 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>-0.0041644240</t>
-        </is>
-      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="n">
-        <v>1.853841414141414</v>
+        <v>1.858665656565657</v>
       </c>
       <c r="O24" t="n">
-        <v>82.64642082429501</v>
+        <v>64.40129449838199</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>17443</v>
+        <v>12898</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44622.56597222222</v>
+        <v>44606.78472222222</v>
       </c>
       <c r="C25" t="n">
-        <v>1646228399999</v>
+        <v>1644864899999</v>
       </c>
       <c r="D25" t="n">
-        <v>1.9863</v>
+        <v>1.916</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1735,19 +1647,19 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1426.170631724777</v>
+        <v>1232.493065184936</v>
       </c>
       <c r="G25" t="n">
-        <v>1.978386454183267</v>
+        <v>1.913130304543185</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="J25" t="n">
-        <v>1.004</v>
+        <v>1.0015</v>
       </c>
       <c r="K25" t="n">
         <v>1.02</v>
@@ -1757,68 +1669,256 @@
           <t>normaltrend</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>-0.0037416894</t>
-        </is>
-      </c>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="n">
-        <v>1.990810101010101</v>
+        <v>1.917948484848485</v>
       </c>
       <c r="O25" t="n">
-        <v>29.74828375286042</v>
+        <v>31.6017316017313</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
+        <v>14115</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>44611.01041666666</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1645229999999</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.8763</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>myBuy</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>656.2178467138901</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.87911445</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>normaltrend</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="n">
+        <v>1.873607070707071</v>
+      </c>
+      <c r="O26" t="n">
+        <v>63.22314049586774</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>14213</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>44611.35069444445</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1645259399999</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.888</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>mySell</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>1237.939294595825</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.885172241637544</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>normaltrend</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="n">
+        <v>1.889446464646465</v>
+      </c>
+      <c r="O27" t="n">
+        <v>24.09638554216809</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>14305</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>44611.67013888889</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1645286999999</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.8669</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>myBuy</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>662.4363025728595</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.86970035</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>normaltrend</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="n">
+        <v>1.853841414141414</v>
+      </c>
+      <c r="O28" t="n">
+        <v>82.64642082429501</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>17443</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>44622.56597222222</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1646228399999</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.9863</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>mySell</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>1314.797227800471</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.983325012481278</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>normaltrend</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="n">
+        <v>1.990810101010101</v>
+      </c>
+      <c r="O29" t="n">
+        <v>29.74828375286042</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
         <v>17651</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B30" s="2" t="n">
         <v>44623.28819444445</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C30" t="n">
         <v>1646290799999</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D30" t="n">
         <v>1.9462</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>myBuy</t>
         </is>
       </c>
-      <c r="F26" t="n">
-        <v>732.0653518486541</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1.9539848</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" t="n">
-        <v>1.004</v>
-      </c>
-      <c r="J26" t="n">
-        <v>1.004</v>
-      </c>
-      <c r="K26" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>normaltrend</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>-0.0035095382</t>
-        </is>
-      </c>
-      <c r="N26" t="n">
+      <c r="F30" t="n">
+        <v>674.8964491123628</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.9491193</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1.0015</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>normaltrend</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="n">
         <v>1.944883838383839</v>
       </c>
-      <c r="O26" t="n">
+      <c r="O30" t="n">
         <v>68.37532580364908</v>
       </c>
     </row>

</xml_diff>